<commit_message>
implement ItemFactory, some configurations and finalize Machines
</commit_message>
<xml_diff>
--- a/GameTechTree.xlsx
+++ b/GameTechTree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartul\Documents\TheExiledOnes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7321E33E-E3F0-400E-B9D3-0B4B2A1B3C31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8444F75-8C38-43FF-AB84-FFEDBDC7CBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,30 +445,9 @@
     <t>Alloying Silver, Gold and soul fragments.</t>
   </si>
   <si>
-    <t>iron+silver</t>
-  </si>
-  <si>
-    <t>steel+gold</t>
-  </si>
-  <si>
-    <t>felsteel+electrum</t>
-  </si>
-  <si>
-    <t>cursed steel + cursed electrum</t>
-  </si>
-  <si>
     <t>branch + rock + iron</t>
   </si>
   <si>
-    <t>wood+rock+steel</t>
-  </si>
-  <si>
-    <t>felwood+felstone+felsteel</t>
-  </si>
-  <si>
-    <t>cursewood+cursed stone+cursed steel</t>
-  </si>
-  <si>
     <t>Speed</t>
   </si>
   <si>
@@ -502,15 +481,6 @@
     <t>Cursed Electrum IV</t>
   </si>
   <si>
-    <t>Electrum III</t>
-  </si>
-  <si>
-    <t>Gold II</t>
-  </si>
-  <si>
-    <t>Silver I</t>
-  </si>
-  <si>
     <t>Iron I</t>
   </si>
   <si>
@@ -779,6 +749,36 @@
   </si>
   <si>
     <t>Study</t>
+  </si>
+  <si>
+    <t>Gold III</t>
+  </si>
+  <si>
+    <t>Silver II</t>
+  </si>
+  <si>
+    <t>Copper I</t>
+  </si>
+  <si>
+    <t>iron+copper</t>
+  </si>
+  <si>
+    <t>steel+silver+Mechanism I</t>
+  </si>
+  <si>
+    <t>felsteel+gold+Mechanism II</t>
+  </si>
+  <si>
+    <t>cursed steel + cursed electrum+Mechanism III</t>
+  </si>
+  <si>
+    <t>felwood+felstone+felsteel+Frame II</t>
+  </si>
+  <si>
+    <t>wood+rock+steel+Frame I</t>
+  </si>
+  <si>
+    <t>cursewood+cursed stone+cursed steel+Frame III</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -1592,7 +1592,7 @@
         <v>8</v>
       </c>
       <c r="I26" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="J26" t="s">
         <v>28</v>
@@ -1711,7 +1711,7 @@
         <v>106</v>
       </c>
       <c r="J33" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="K33" t="s">
         <v>84</v>
@@ -1722,10 +1722,10 @@
         <v>74</v>
       </c>
       <c r="H34" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="J34" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="K34" t="s">
         <v>85</v>
@@ -1922,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52704A77-CCC3-48DA-AB7C-9B77A5FEAF60}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
         <v>122</v>
@@ -1955,24 +1955,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>126</v>
@@ -1985,24 +1985,24 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>128</v>
@@ -2015,24 +2015,24 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>130</v>
@@ -2045,19 +2045,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>157</v>
+        <v>240</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>155</v>
+        <v>238</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2077,7 +2077,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B12" t="s">
         <v>122</v>
@@ -2094,171 +2094,171 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>136</v>
+        <v>241</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>242</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>243</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>246</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>245</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E20" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
         <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E24" t="s">
         <v>121</v>
@@ -2266,70 +2266,70 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" t="s">
         <v>210</v>
       </c>
-      <c r="D25" t="s">
-        <v>220</v>
-      </c>
       <c r="E25" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D26" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E26" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D27" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E27" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E28" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2369,7 +2369,7 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
         <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,7 +2393,7 @@
         <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2401,15 +2401,15 @@
         <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2433,7 +2433,7 @@
         <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement Use Hand basic tool, Crafting Result fel consumption
</commit_message>
<xml_diff>
--- a/GameTechTree.xlsx
+++ b/GameTechTree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartul\Documents\TheExiledOnes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8444F75-8C38-43FF-AB84-FFEDBDC7CBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9565D2E1-681D-4946-93A4-853E39136FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="60" windowWidth="19890" windowHeight="14190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
start on Automaton implementation
</commit_message>
<xml_diff>
--- a/GameTechTree.xlsx
+++ b/GameTechTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wc3-projects\TheExiledOnes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB62184-CF71-4967-A53D-66B08B8E3769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D14635-0A16-4F10-8AC9-D5E588BC71E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2515,7 +2515,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add multiple abilities, experience progress
</commit_message>
<xml_diff>
--- a/GameTechTree.xlsx
+++ b/GameTechTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wc3-projects\TheExiledOnes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64A6BC9-34A5-4239-BDB6-5D04754B851D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD543A-4FB5-44D7-9A58-FAD01297C79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="266">
   <si>
     <t>Prospector</t>
   </si>
@@ -819,6 +819,21 @@
   </si>
   <si>
     <t>Net</t>
+  </si>
+  <si>
+    <t>2x Iron, 2x Log, Rabbit + Frog</t>
+  </si>
+  <si>
+    <t>Frame + Iron, Copper + Frog,  Skink + Rabbit</t>
+  </si>
+  <si>
+    <t>Tanks</t>
+  </si>
+  <si>
+    <t>Converters</t>
+  </si>
+  <si>
+    <t>4 Iron, 4 Iron, 3 Iron + Frame</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52704A77-CCC3-48DA-AB7C-9B77A5FEAF60}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2539,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,7 +2565,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>235</v>
       </c>
       <c r="F3" t="s">
         <v>258</v>
@@ -2642,62 +2657,83 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>263</v>
+      </c>
+      <c r="D19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
finish implementation of item transfer node manager
</commit_message>
<xml_diff>
--- a/GameTechTree.xlsx
+++ b/GameTechTree.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wc3-projects\TheExiledOnes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5B166E-0BC9-4E78-AF4F-8B1BF828FA47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5620D4-8A56-46D2-94CA-06D842F8B110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Unit stats" sheetId="5" r:id="rId4"/>
+    <sheet name="Artisan" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="301">
   <si>
     <t>Prospector</t>
   </si>
@@ -898,6 +899,48 @@
   </si>
   <si>
     <t>Pick</t>
+  </si>
+  <si>
+    <t>Crude Pickaxe</t>
+  </si>
+  <si>
+    <t>Mineshaft</t>
+  </si>
+  <si>
+    <t>Furnace</t>
+  </si>
+  <si>
+    <t>To Automate:</t>
+  </si>
+  <si>
+    <t>Stone mining</t>
+  </si>
+  <si>
+    <t>Log mining</t>
+  </si>
+  <si>
+    <t>Quarry</t>
+  </si>
+  <si>
+    <t>Mutator</t>
+  </si>
+  <si>
+    <t>Steel processing</t>
+  </si>
+  <si>
+    <t>Foundry</t>
+  </si>
+  <si>
+    <t>Extract Fel</t>
+  </si>
+  <si>
+    <t>Transfer Fel</t>
+  </si>
+  <si>
+    <t>Scouts</t>
+  </si>
+  <si>
+    <t>Assembler</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1011,6 +1054,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -2062,7 +2108,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,7 +2650,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,8 +2858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1474709D-14AD-4F9F-8D7D-D4B71FDDB310}">
   <dimension ref="A3:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,4 +3087,316 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5A426C-8924-4C1E-B3C0-0631FAC30DBE}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>297</v>
+      </c>
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" t="s">
+        <v>299</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>231</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>298</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>289</v>
+      </c>
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>263</v>
+      </c>
+      <c r="D19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>291</v>
+      </c>
+      <c r="E34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>292</v>
+      </c>
+      <c r="E35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>295</v>
+      </c>
+      <c r="E36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>